<commit_message>
Cahier des charges fini
</commit_message>
<xml_diff>
--- a/Documentation/Journal_de_travail_I_Shoes.xlsx
+++ b/Documentation/Journal_de_travail_I_Shoes.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\romai\Romain\GitHub DATA\I_Shoes\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sacha.JACCARD\Documents\GitHub\I_Shoes\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{396E043C-9206-47DF-9B5C-A77EBB956BD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7680" yWindow="1200" windowWidth="15510" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7680" yWindow="1200" windowWidth="15510" windowHeight="11295"/>
   </bookViews>
   <sheets>
     <sheet name="Journal_de_travail" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="21">
   <si>
     <t>Date</t>
   </si>
@@ -102,11 +101,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="hh:mm:ss;@"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -157,6 +156,12 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="8"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -179,7 +184,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -219,12 +224,27 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="6">
+    <dxf>
+      <font>
+        <color theme="7"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -256,16 +276,6 @@
     <dxf>
       <numFmt numFmtId="164" formatCode="hh:mm:ss;@"/>
     </dxf>
-    <dxf>
-      <font>
-        <color theme="7"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9"/>
-      </font>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -280,22 +290,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="A1:H1006" totalsRowShown="0">
-  <autoFilter ref="A1:H1006" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:H1007" totalsRowShown="0">
+  <autoFilter ref="A1:H1007"/>
+  <sortState ref="A2:H3">
     <sortCondition ref="A1:A6"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Début" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Fin" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Durée" dataDxfId="1">
+    <tableColumn id="1" name="Date"/>
+    <tableColumn id="2" name="Début" dataDxfId="5"/>
+    <tableColumn id="3" name="Fin" dataDxfId="4"/>
+    <tableColumn id="4" name="Durée" dataDxfId="3">
       <calculatedColumnFormula>SUM(Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Thème"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Nom de présence"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Description"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Sources" dataDxfId="0"/>
+    <tableColumn id="5" name="Thème"/>
+    <tableColumn id="6" name="Nom de présence"/>
+    <tableColumn id="7" name="Description"/>
+    <tableColumn id="8" name="Sources" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -563,11 +573,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1102"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J1103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -606,44 +616,38 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="18">
         <v>44959</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="1">
         <v>0.5625</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2" s="1">
+        <v>0.62152777777777779</v>
+      </c>
+      <c r="D2" s="17">
+        <f>SUM(Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]])</f>
+        <v>5.902777777777779E-2</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="14"/>
+    </row>
+    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>44959</v>
+      </c>
+      <c r="B3" s="5">
+        <v>0.5625</v>
+      </c>
+      <c r="C3" s="8">
         <v>0.64583333333333337</v>
       </c>
-      <c r="D2" s="9">
+      <c r="D3" s="9">
         <f>SUM(Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]])</f>
         <v>8.333333333333337E-2</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="10"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="7">
-        <v>44959</v>
-      </c>
-      <c r="B3" s="8">
-        <v>0.65625</v>
-      </c>
-      <c r="C3" s="8">
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="D3" s="9">
-        <f>SUM(Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]])</f>
-        <v>1.041666666666663E-2</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>12</v>
@@ -652,23 +656,23 @@
         <v>7</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" s="11"/>
+        <v>13</v>
+      </c>
+      <c r="H3" s="10"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>44959</v>
       </c>
       <c r="B4" s="8">
+        <v>0.65625</v>
+      </c>
+      <c r="C4" s="8">
         <v>0.66666666666666663</v>
       </c>
-      <c r="C4" s="8">
-        <v>0.6875</v>
-      </c>
       <c r="D4" s="9">
         <f>SUM(Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]])</f>
-        <v>2.083333333333337E-2</v>
+        <v>1.041666666666663E-2</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>12</v>
@@ -677,23 +681,23 @@
         <v>7</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H4" s="16"/>
-    </row>
-    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="H4" s="11"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>44959</v>
       </c>
       <c r="B5" s="8">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C5" s="8">
         <v>0.6875</v>
       </c>
-      <c r="C5" s="8">
-        <v>0.70486111111111116</v>
-      </c>
       <c r="D5" s="9">
         <f>SUM(Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]])</f>
-        <v>1.736111111111116E-2</v>
+        <v>2.083333333333337E-2</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>12</v>
@@ -702,23 +706,23 @@
         <v>7</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" s="11"/>
-    </row>
-    <row r="6" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="H5" s="16"/>
+    </row>
+    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
-        <v>44961</v>
+        <v>44959</v>
       </c>
       <c r="B6" s="8">
-        <v>0.67013888888888884</v>
+        <v>0.6875</v>
       </c>
       <c r="C6" s="8">
         <v>0.70486111111111116</v>
       </c>
       <c r="D6" s="9">
         <f>SUM(Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]])</f>
-        <v>3.4722222222222321E-2</v>
+        <v>1.736111111111116E-2</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>12</v>
@@ -727,23 +731,23 @@
         <v>7</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="H6" s="12"/>
-    </row>
-    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="H6" s="11"/>
+    </row>
+    <row r="7" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>44961</v>
       </c>
       <c r="B7" s="8">
-        <v>0.70833333333333337</v>
+        <v>0.67013888888888884</v>
       </c>
       <c r="C7" s="8">
-        <v>0.95833333333333337</v>
+        <v>0.70486111111111116</v>
       </c>
       <c r="D7" s="9">
         <f>SUM(Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]])</f>
-        <v>0.25</v>
+        <v>3.4722222222222321E-2</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>12</v>
@@ -752,48 +756,59 @@
         <v>7</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="H7" s="11"/>
-    </row>
-    <row r="8" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="H7" s="12"/>
+    </row>
+    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
-        <v>44962</v>
+        <v>44961</v>
       </c>
       <c r="B8" s="8">
-        <v>0.34027777777777773</v>
+        <v>0.70833333333333337</v>
       </c>
       <c r="C8" s="8">
-        <v>0.4236111111111111</v>
+        <v>0.95833333333333337</v>
       </c>
       <c r="D8" s="9">
         <f>SUM(Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]])</f>
-        <v>8.333333333333337E-2</v>
+        <v>0.25</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>7</v>
       </c>
       <c r="G8" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="11"/>
+    </row>
+    <row r="9" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
+        <v>44962</v>
+      </c>
+      <c r="B9" s="8">
+        <v>0.34027777777777773</v>
+      </c>
+      <c r="C9" s="8">
+        <v>0.4236111111111111</v>
+      </c>
+      <c r="D9" s="9">
+        <f>SUM(Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]])</f>
+        <v>8.333333333333337E-2</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="H8" s="11"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="9">
-        <f>SUM(Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]])</f>
-        <v>0</v>
-      </c>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="3"/>
+      <c r="H9" s="11"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
@@ -806,8 +821,8 @@
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="6"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="3"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
@@ -821,6 +836,7 @@
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
       <c r="H11" s="11"/>
+      <c r="I11" s="6"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
@@ -872,7 +888,7 @@
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
-      <c r="H15" s="13"/>
+      <c r="H15" s="11"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
@@ -924,9 +940,7 @@
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
+      <c r="H19" s="13"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
@@ -954,7 +968,9 @@
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
-      <c r="H21" s="13"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
@@ -1032,7 +1048,7 @@
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
-      <c r="H27" s="12"/>
+      <c r="H27" s="13"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
@@ -1045,7 +1061,7 @@
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
       <c r="G28" s="6"/>
-      <c r="H28" s="13"/>
+      <c r="H28" s="12"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="7"/>
@@ -1175,7 +1191,7 @@
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
-      <c r="H38" s="11"/>
+      <c r="H38" s="13"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="7"/>
@@ -1188,8 +1204,7 @@
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
-      <c r="H39" s="12"/>
-      <c r="I39" s="13"/>
+      <c r="H39" s="11"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
@@ -1202,7 +1217,8 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
-      <c r="H40" s="6"/>
+      <c r="H40" s="12"/>
+      <c r="I40" s="13"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
@@ -1215,7 +1231,7 @@
       <c r="E41" s="6"/>
       <c r="F41" s="6"/>
       <c r="G41" s="6"/>
-      <c r="H41" s="11"/>
+      <c r="H41" s="6"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="7"/>
@@ -1229,7 +1245,6 @@
       <c r="F42" s="6"/>
       <c r="G42" s="6"/>
       <c r="H42" s="11"/>
-      <c r="I42" s="6"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="7"/>
@@ -1242,8 +1257,8 @@
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="12"/>
-      <c r="I43" s="13"/>
+      <c r="H43" s="11"/>
+      <c r="I43" s="6"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="7"/>
@@ -1256,7 +1271,8 @@
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="11"/>
+      <c r="H44" s="12"/>
+      <c r="I44" s="13"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="7"/>
@@ -1269,7 +1285,7 @@
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="13"/>
+      <c r="H45" s="11"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="7"/>
@@ -1282,7 +1298,7 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="11"/>
+      <c r="H46" s="13"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="7"/>
@@ -1295,7 +1311,7 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="12"/>
+      <c r="H47" s="11"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="7"/>
@@ -1308,7 +1324,7 @@
       <c r="E48" s="6"/>
       <c r="F48" s="6"/>
       <c r="G48" s="6"/>
-      <c r="H48" s="13"/>
+      <c r="H48" s="12"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="7"/>
@@ -1334,8 +1350,7 @@
       <c r="E50" s="6"/>
       <c r="F50" s="6"/>
       <c r="G50" s="6"/>
-      <c r="H50" s="12"/>
-      <c r="I50" s="11"/>
+      <c r="H50" s="13"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="7"/>
@@ -1348,7 +1363,8 @@
       <c r="E51" s="6"/>
       <c r="F51" s="6"/>
       <c r="G51" s="6"/>
-      <c r="H51" s="13"/>
+      <c r="H51" s="12"/>
+      <c r="I51" s="11"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="7"/>
@@ -1387,8 +1403,7 @@
       <c r="E54" s="6"/>
       <c r="F54" s="6"/>
       <c r="G54" s="6"/>
-      <c r="H54" s="12"/>
-      <c r="I54" s="11"/>
+      <c r="H54" s="13"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="7"/>
@@ -1401,7 +1416,8 @@
       <c r="E55" s="6"/>
       <c r="F55" s="6"/>
       <c r="G55" s="6"/>
-      <c r="H55" s="14"/>
+      <c r="H55" s="12"/>
+      <c r="I55" s="11"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="7"/>
@@ -1453,8 +1469,7 @@
       <c r="E59" s="6"/>
       <c r="F59" s="6"/>
       <c r="G59" s="6"/>
-      <c r="H59" s="12"/>
-      <c r="I59" s="6"/>
+      <c r="H59" s="14"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="7"/>
@@ -1467,7 +1482,8 @@
       <c r="E60" s="6"/>
       <c r="F60" s="6"/>
       <c r="G60" s="6"/>
-      <c r="H60" s="14"/>
+      <c r="H60" s="12"/>
+      <c r="I60" s="6"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="7"/>
@@ -1506,7 +1522,7 @@
       <c r="E63" s="6"/>
       <c r="F63" s="6"/>
       <c r="G63" s="6"/>
-      <c r="H63" s="12"/>
+      <c r="H63" s="14"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="7"/>
@@ -1519,7 +1535,7 @@
       <c r="E64" s="6"/>
       <c r="F64" s="6"/>
       <c r="G64" s="6"/>
-      <c r="H64" s="11"/>
+      <c r="H64" s="12"/>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="7"/>
@@ -1532,7 +1548,7 @@
       <c r="E65" s="6"/>
       <c r="F65" s="6"/>
       <c r="G65" s="6"/>
-      <c r="H65" s="12"/>
+      <c r="H65" s="11"/>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="7"/>
@@ -1545,7 +1561,7 @@
       <c r="E66" s="6"/>
       <c r="F66" s="6"/>
       <c r="G66" s="6"/>
-      <c r="H66" s="11"/>
+      <c r="H66" s="12"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="7"/>
@@ -1558,7 +1574,7 @@
       <c r="E67" s="6"/>
       <c r="F67" s="6"/>
       <c r="G67" s="6"/>
-      <c r="H67" s="15"/>
+      <c r="H67" s="11"/>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="7"/>
@@ -1584,7 +1600,7 @@
       <c r="E69" s="6"/>
       <c r="F69" s="6"/>
       <c r="G69" s="6"/>
-      <c r="H69" s="14"/>
+      <c r="H69" s="15"/>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="7"/>
@@ -1600,10 +1616,16 @@
       <c r="H70" s="14"/>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71" s="7"/>
+      <c r="B71" s="8"/>
+      <c r="C71" s="8"/>
       <c r="D71" s="9">
         <f>SUM(Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]])</f>
         <v>0</v>
       </c>
+      <c r="E71" s="6"/>
+      <c r="F71" s="6"/>
+      <c r="G71" s="6"/>
       <c r="H71" s="14"/>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
@@ -8152,8 +8174,11 @@
       <c r="H1006" s="14"/>
     </row>
     <row r="1007" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D1007" s="2"/>
-      <c r="H1007" s="3"/>
+      <c r="D1007" s="9">
+        <f>SUM(Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]])</f>
+        <v>0</v>
+      </c>
+      <c r="H1007" s="14"/>
     </row>
     <row r="1008" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D1008" s="2"/>
@@ -8376,6 +8401,7 @@
       <c r="H1062" s="3"/>
     </row>
     <row r="1063" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D1063" s="2"/>
       <c r="H1063" s="3"/>
     </row>
     <row r="1064" spans="4:8" x14ac:dyDescent="0.25">
@@ -8484,40 +8510,43 @@
       <c r="H1098" s="3"/>
     </row>
     <row r="1099" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1099" t="s">
-        <v>8</v>
-      </c>
+      <c r="H1099" s="3"/>
     </row>
     <row r="1100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1100" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="1101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1101" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="1102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1102" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1103" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1103" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="timePeriod" dxfId="5" priority="1" timePeriod="today">
+    <cfRule type="timePeriod" dxfId="1" priority="1" timePeriod="today">
       <formula>FLOOR(A1,1)=TODAY()</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="4" priority="2" timePeriod="yesterday">
+    <cfRule type="timePeriod" dxfId="0" priority="2" timePeriod="yesterday">
       <formula>FLOOR(A1,1)=TODAY()-1</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
-      <formula1>$A$1100:$A$1102</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F1048576">
+      <formula1>$A$1101:$A$1103</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1098" xr:uid="{00000000-0002-0000-0000-000001000000}">
-      <formula1>$A$1100:$A$1101</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1099">
+      <formula1>$A$1101:$A$1102</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>